<commit_message>
Updated single step linear
Single step linear can now have its input file defined in the code.
Also, it is confirmed that the other test files work for it, and it is
stored within the greater single step file.
</commit_message>
<xml_diff>
--- a/Linear Single Step/input.xlsx
+++ b/Linear Single Step/input.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950"/>
+    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sources" sheetId="1" r:id="rId1"/>
@@ -368,12 +368,6 @@
     <t>SubEff1</t>
   </si>
   <si>
-    <t>In</t>
-  </si>
-  <si>
-    <t>Out</t>
-  </si>
-  <si>
     <t>EnergyType</t>
   </si>
   <si>
@@ -576,6 +570,12 @@
   </si>
   <si>
     <t>OutMax</t>
+  </si>
+  <si>
+    <t>From</t>
+  </si>
+  <si>
+    <t>To</t>
   </si>
 </sst>
 </file>
@@ -931,7 +931,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
@@ -951,27 +951,27 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
         <v>14</v>
       </c>
-      <c r="C1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" t="s">
-        <v>16</v>
-      </c>
       <c r="F1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="G1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -980,7 +980,7 @@
         <v>0.01</v>
       </c>
       <c r="D2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E2">
         <v>7.3200000000000001E-2</v>
@@ -994,7 +994,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -1003,7 +1003,7 @@
         <v>0.02</v>
       </c>
       <c r="D3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -1017,7 +1017,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -1026,7 +1026,7 @@
         <v>0.05</v>
       </c>
       <c r="D4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E4">
         <v>0</v>
@@ -1066,21 +1066,21 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
         <v>15</v>
-      </c>
-      <c r="D1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -1089,7 +1089,7 @@
         <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E2">
         <v>858</v>
@@ -1097,7 +1097,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -1106,7 +1106,7 @@
         <v>0</v>
       </c>
       <c r="D3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E3">
         <v>7.5</v>
@@ -1114,7 +1114,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -1123,7 +1123,7 @@
         <v>0</v>
       </c>
       <c r="D4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E4">
         <v>24.2</v>
@@ -1131,7 +1131,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -1140,7 +1140,7 @@
         <v>0</v>
       </c>
       <c r="D5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E5">
         <v>130.30000000000001</v>
@@ -1148,7 +1148,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -1157,7 +1157,7 @@
         <v>0</v>
       </c>
       <c r="D6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E6">
         <v>414.5</v>
@@ -1206,37 +1206,37 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="H1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J1" t="s">
         <v>26</v>
       </c>
-      <c r="I1" t="s">
-        <v>27</v>
-      </c>
-      <c r="J1" t="s">
-        <v>28</v>
-      </c>
       <c r="K1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="L1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="M1" t="s">
         <v>2</v>
@@ -1245,15 +1245,15 @@
         <v>3</v>
       </c>
       <c r="O1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="P1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -1271,19 +1271,19 @@
         <v>999999</v>
       </c>
       <c r="G2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H2">
         <v>1</v>
       </c>
       <c r="K2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="L2">
         <v>0.33</v>
       </c>
       <c r="M2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="N2">
         <v>0.67</v>
@@ -1291,7 +1291,7 @@
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -1309,13 +1309,13 @@
         <v>999999</v>
       </c>
       <c r="G3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H3">
         <v>1</v>
       </c>
       <c r="K3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="L3">
         <v>1</v>
@@ -1323,7 +1323,7 @@
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -1341,13 +1341,13 @@
         <v>999999</v>
       </c>
       <c r="G4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H4">
         <v>1</v>
       </c>
       <c r="K4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="L4">
         <v>1</v>
@@ -1355,7 +1355,7 @@
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -1373,13 +1373,13 @@
         <v>999999</v>
       </c>
       <c r="G5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="H5">
         <v>1</v>
       </c>
       <c r="K5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="L5">
         <v>1</v>
@@ -1387,7 +1387,7 @@
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -1405,13 +1405,13 @@
         <v>999999</v>
       </c>
       <c r="G6" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="H6">
         <v>1</v>
       </c>
       <c r="K6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="L6">
         <v>1</v>
@@ -1419,7 +1419,7 @@
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -1438,13 +1438,13 @@
         <v>999999</v>
       </c>
       <c r="G7" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="H7">
         <v>1</v>
       </c>
       <c r="K7" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="L7">
         <v>1</v>
@@ -1452,7 +1452,7 @@
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -1471,13 +1471,13 @@
         <v>999999</v>
       </c>
       <c r="G8" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H8">
         <v>1</v>
       </c>
       <c r="K8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="L8">
         <v>1</v>
@@ -1485,7 +1485,7 @@
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -1504,13 +1504,13 @@
         <v>999999</v>
       </c>
       <c r="G9" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H9">
         <v>1</v>
       </c>
       <c r="K9" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="L9">
         <v>1</v>
@@ -1518,7 +1518,7 @@
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -1537,13 +1537,13 @@
         <v>999999</v>
       </c>
       <c r="G10" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H10">
         <v>1</v>
       </c>
       <c r="K10" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="L10">
         <v>1</v>
@@ -1551,7 +1551,7 @@
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -1570,13 +1570,13 @@
         <v>999999</v>
       </c>
       <c r="G11" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H11">
         <v>1</v>
       </c>
       <c r="K11" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="L11">
         <v>1</v>
@@ -1584,7 +1584,7 @@
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -1603,13 +1603,13 @@
         <v>999999</v>
       </c>
       <c r="G12" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H12">
         <v>1</v>
       </c>
       <c r="K12" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="L12">
         <v>1</v>
@@ -1625,8 +1625,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1640,335 +1640,335 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D1" t="s">
         <v>4</v>
-      </c>
-      <c r="C1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D6" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C7" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D7" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C8" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D8" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B9" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C9" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D9" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B10" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C10" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D10" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B11" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C11" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D11" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C12" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D12" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B13" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C13" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D13" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B14" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C14" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D14" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B15" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C15" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D15" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B16" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C16" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D16" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B17" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C17" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D17" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B18" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C18" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D18" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B19" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C19" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D19" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B20" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C20" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D20" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B21" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C21" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D21" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B22" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C22" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D22" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B23" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C23" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D23" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B24" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C24" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D24" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -1991,21 +1991,21 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -2016,10 +2016,10 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -2045,7 +2045,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>